<commit_message>
Designed the notallowed page and the homepage has a reviewed design also 001.
</commit_message>
<xml_diff>
--- a/public/2025 final biocoding.xlsx
+++ b/public/2025 final biocoding.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7755"/>
+    <workbookView windowWidth="20490" windowHeight="8205"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
     <t xml:space="preserve">Chimezie Igwegbe Nzoputam </t>
   </si>
   <si>
-    <t>Chioma Deborah Nzeduru æ</t>
+    <t>Chioma Deborah Nzeduru</t>
   </si>
   <si>
     <t xml:space="preserve">Christopher Ogheneruemu Ofuadarho </t>
@@ -1345,7 +1345,7 @@
   <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Services and Consults came for their certificate today...
</commit_message>
<xml_diff>
--- a/public/2025 final biocoding.xlsx
+++ b/public/2025 final biocoding.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7755"/>
+    <workbookView windowWidth="20475" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1380,8 +1380,8 @@
   <sheetPr/>
   <dimension ref="A1:A39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Certificate for the trip to Imo State.
</commit_message>
<xml_diff>
--- a/public/2025 final biocoding.xlsx
+++ b/public/2025 final biocoding.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20475" windowHeight="7770"/>
+    <workbookView windowWidth="20490" windowHeight="8205"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
     <t>Musa Sani</t>
   </si>
   <si>
-    <t xml:space="preserve">Eben Leonel Albano Maiopué </t>
+    <t>Eben Leonel Albano Maiopué</t>
   </si>
   <si>
     <t>JOSEPH ALALE AWEEYA</t>

</xml_diff>